<commit_message>
Update '外籍學者' to '境外學者' of example excel files.
</commit_message>
<xml_diff>
--- a/public/Excel_example/prof/foreign_prof_attend_conference.xlsx
+++ b/public/Excel_example/prof/foreign_prof_attend_conference.xlsx
@@ -31,10 +31,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>外籍學者身分（教授、副教授、助理教授或博士後研究員）</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>國籍</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -52,6 +48,10 @@
   </si>
   <si>
     <t>結束時間</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>境外學者身分（教授、副教授、助理教授或博士後研究員）</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -427,7 +427,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -452,22 +452,22 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>0</v>

</xml_diff>